<commit_message>
Temporarily fixed aspect ratio issue in safari, though need better solution later
</commit_message>
<xml_diff>
--- a/public/food-data.xlsx
+++ b/public/food-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanau/WebstormProjects/nutrition-calculator/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0363C207-F3F6-1146-8D1E-3B014C09C11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A873AF-6DDE-7546-A2E0-1400DA68C1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="740" windowWidth="29400" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="300 Common Foods - editing" sheetId="1" r:id="rId1"/>
@@ -5174,7 +5174,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="V5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AF10" sqref="AF10"/>
+      <selection pane="bottomRight" activeCell="AH38" sqref="AH38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Switched language to chinese
</commit_message>
<xml_diff>
--- a/public/food-data.xlsx
+++ b/public/food-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanau/WebstormProjects/nutrition-calculator/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342BCCF6-D836-D24D-91BE-3D999E64EE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AA3DFC-AAF1-D84E-9F50-E9162A145801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -297,7 +297,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3216" uniqueCount="1368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3216" uniqueCount="1359">
   <si>
     <t>WeRise Nutrition Calculator Database</t>
   </si>
@@ -4374,33 +4374,6 @@
   </si>
   <si>
     <t>1TmlG0MixbxwTf-8pRtcevu9nJ0xpcb_G</t>
-  </si>
-  <si>
-    <t>Dine Out Dishes</t>
-  </si>
-  <si>
-    <t>HK Delicacies</t>
-  </si>
-  <si>
-    <t>Beverages</t>
-  </si>
-  <si>
-    <t>Breakfast Foods</t>
-  </si>
-  <si>
-    <t>Snacks</t>
-  </si>
-  <si>
-    <t>HK Bakery</t>
-  </si>
-  <si>
-    <t>HK Desserts</t>
-  </si>
-  <si>
-    <t>Condiments</t>
-  </si>
-  <si>
-    <t>Fruits</t>
   </si>
 </sst>
 </file>
@@ -5383,10 +5356,10 @@
   <dimension ref="A1:BB1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="F325" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="F121" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F129" sqref="F129"/>
+      <selection pane="bottomRight" activeCell="AE92" sqref="AE92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -5672,7 +5645,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>29</v>
@@ -5801,7 +5774,7 @@
         <v>38</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>39</v>
@@ -5929,7 +5902,7 @@
     <row r="7" spans="1:54" ht="14.25" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>43</v>
@@ -6056,7 +6029,7 @@
     <row r="8" spans="1:54" ht="14.25" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>48</v>
@@ -6187,7 +6160,7 @@
         <v>51</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>52</v>
@@ -6318,7 +6291,7 @@
         <v>51</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>56</v>
@@ -6435,7 +6408,7 @@
     <row r="11" spans="1:54" ht="14.25" customHeight="1" thickBot="1">
       <c r="A11" s="1"/>
       <c r="B11" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>60</v>
@@ -6554,7 +6527,7 @@
         <v>64</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>65</v>
@@ -6675,7 +6648,7 @@
     <row r="13" spans="1:54" ht="14.25" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>67</v>
@@ -6800,7 +6773,7 @@
     <row r="14" spans="1:54" ht="14.25" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>70</v>
@@ -6925,7 +6898,7 @@
     <row r="15" spans="1:54" ht="14.25" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C15" s="41" t="s">
         <v>74</v>
@@ -7050,7 +7023,7 @@
     <row r="16" spans="1:54" ht="14.25" customHeight="1" thickBot="1">
       <c r="A16" s="1"/>
       <c r="B16" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>76</v>
@@ -7175,7 +7148,7 @@
     <row r="17" spans="1:54" ht="14.25" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>79</v>
@@ -7294,7 +7267,7 @@
     <row r="18" spans="1:54" ht="14.25" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>82</v>
@@ -7411,7 +7384,7 @@
     <row r="19" spans="1:54" ht="14.25" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>84</v>
@@ -7528,7 +7501,7 @@
     <row r="20" spans="1:54" ht="14.25" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>86</v>
@@ -7645,7 +7618,7 @@
     <row r="21" spans="1:54" ht="14.25" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>88</v>
@@ -7762,7 +7735,7 @@
     <row r="22" spans="1:54" ht="14.25" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>90</v>
@@ -7879,7 +7852,7 @@
     <row r="23" spans="1:54" ht="14.25" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>92</v>
@@ -7996,7 +7969,7 @@
     <row r="24" spans="1:54" ht="14.25" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>94</v>
@@ -8113,7 +8086,7 @@
     <row r="25" spans="1:54" ht="14.25" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>96</v>
@@ -8230,7 +8203,7 @@
     <row r="26" spans="1:54" ht="14.25" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C26" s="41" t="s">
         <v>98</v>
@@ -8347,7 +8320,7 @@
     <row r="27" spans="1:54" ht="14.25" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C27" s="41" t="s">
         <v>100</v>
@@ -8464,7 +8437,7 @@
     <row r="28" spans="1:54" ht="14.25" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>102</v>
@@ -8581,7 +8554,7 @@
     <row r="29" spans="1:54" ht="14.25" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>104</v>
@@ -8698,7 +8671,7 @@
     <row r="30" spans="1:54" ht="14.25" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>106</v>
@@ -8815,7 +8788,7 @@
     <row r="31" spans="1:54" ht="14.25" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>108</v>
@@ -8934,7 +8907,7 @@
         <v>110</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>111</v>
@@ -9051,7 +9024,7 @@
     <row r="33" spans="1:54" ht="14.25" customHeight="1">
       <c r="A33" s="2"/>
       <c r="B33" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>114</v>
@@ -9168,7 +9141,7 @@
     <row r="34" spans="1:54" ht="14.25" customHeight="1">
       <c r="A34" s="2"/>
       <c r="B34" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>116</v>
@@ -9285,7 +9258,7 @@
     <row r="35" spans="1:54" ht="14.25" customHeight="1">
       <c r="A35" s="2"/>
       <c r="B35" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>118</v>
@@ -9402,7 +9375,7 @@
     <row r="36" spans="1:54" ht="14.25" customHeight="1">
       <c r="A36" s="2"/>
       <c r="B36" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>120</v>
@@ -9519,7 +9492,7 @@
     <row r="37" spans="1:54" ht="14.25" customHeight="1">
       <c r="A37" s="2"/>
       <c r="B37" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>122</v>
@@ -9636,7 +9609,7 @@
     <row r="38" spans="1:54" ht="14.25" customHeight="1">
       <c r="A38" s="2"/>
       <c r="B38" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>124</v>
@@ -9753,7 +9726,7 @@
     <row r="39" spans="1:54" ht="14.25" customHeight="1">
       <c r="A39" s="2"/>
       <c r="B39" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>126</v>
@@ -9870,7 +9843,7 @@
     <row r="40" spans="1:54" ht="14.25" customHeight="1">
       <c r="A40" s="2"/>
       <c r="B40" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>128</v>
@@ -9987,7 +9960,7 @@
     <row r="41" spans="1:54" ht="14.25" customHeight="1">
       <c r="A41" s="2"/>
       <c r="B41" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>130</v>
@@ -10104,7 +10077,7 @@
     <row r="42" spans="1:54" ht="14.25" customHeight="1">
       <c r="A42" s="2"/>
       <c r="B42" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>132</v>
@@ -10221,7 +10194,7 @@
     <row r="43" spans="1:54" ht="14.25" customHeight="1">
       <c r="A43" s="2"/>
       <c r="B43" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>134</v>
@@ -10338,7 +10311,7 @@
     <row r="44" spans="1:54" ht="14.25" customHeight="1">
       <c r="A44" s="2"/>
       <c r="B44" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>136</v>
@@ -10455,7 +10428,7 @@
     <row r="45" spans="1:54" ht="14.25" customHeight="1">
       <c r="A45" s="2"/>
       <c r="B45" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>139</v>
@@ -10572,7 +10545,7 @@
     <row r="46" spans="1:54" ht="14.25" customHeight="1">
       <c r="A46" s="2"/>
       <c r="B46" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>141</v>
@@ -10689,7 +10662,7 @@
     <row r="47" spans="1:54" ht="14.25" customHeight="1">
       <c r="A47" s="2"/>
       <c r="B47" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>143</v>
@@ -10806,7 +10779,7 @@
     <row r="48" spans="1:54" ht="14.25" customHeight="1">
       <c r="A48" s="2"/>
       <c r="B48" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>145</v>
@@ -10923,7 +10896,7 @@
     <row r="49" spans="1:54" ht="14.25" customHeight="1">
       <c r="A49" s="2"/>
       <c r="B49" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>147</v>
@@ -11039,7 +11012,7 @@
     <row r="50" spans="1:54" ht="14.25" customHeight="1">
       <c r="A50" s="2"/>
       <c r="B50" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>149</v>
@@ -11156,7 +11129,7 @@
     <row r="51" spans="1:54" ht="14.25" customHeight="1">
       <c r="A51" s="2"/>
       <c r="B51" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>151</v>
@@ -11275,7 +11248,7 @@
         <v>153</v>
       </c>
       <c r="B52" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>154</v>
@@ -11392,7 +11365,7 @@
     <row r="53" spans="1:54" ht="14.25" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>156</v>
@@ -11509,7 +11482,7 @@
     <row r="54" spans="1:54" ht="14.25" customHeight="1">
       <c r="A54" s="1"/>
       <c r="B54" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>158</v>
@@ -11626,7 +11599,7 @@
     <row r="55" spans="1:54" ht="14.25" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>160</v>
@@ -11743,7 +11716,7 @@
     <row r="56" spans="1:54" ht="14.25" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>162</v>
@@ -11860,7 +11833,7 @@
     <row r="57" spans="1:54" ht="14.25" customHeight="1">
       <c r="A57" s="1"/>
       <c r="B57" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>164</v>
@@ -11977,7 +11950,7 @@
     <row r="58" spans="1:54" ht="14.25" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>166</v>
@@ -12094,7 +12067,7 @@
     <row r="59" spans="1:54" ht="14.25" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>168</v>
@@ -12211,7 +12184,7 @@
     <row r="60" spans="1:54" ht="14.25" customHeight="1">
       <c r="A60" s="1"/>
       <c r="B60" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>170</v>
@@ -12328,7 +12301,7 @@
     <row r="61" spans="1:54" ht="14.25" customHeight="1">
       <c r="A61" s="1"/>
       <c r="B61" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>172</v>
@@ -12445,7 +12418,7 @@
     <row r="62" spans="1:54" ht="14.25" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>174</v>
@@ -12562,7 +12535,7 @@
     <row r="63" spans="1:54" ht="14.25" customHeight="1">
       <c r="A63" s="1"/>
       <c r="B63" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>176</v>
@@ -12679,7 +12652,7 @@
     <row r="64" spans="1:54" ht="14.25" customHeight="1">
       <c r="A64" s="1"/>
       <c r="B64" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>178</v>
@@ -12796,7 +12769,7 @@
     <row r="65" spans="1:54" ht="14.25" customHeight="1">
       <c r="A65" s="1"/>
       <c r="B65" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>180</v>
@@ -12913,7 +12886,7 @@
     <row r="66" spans="1:54" ht="14.25" customHeight="1">
       <c r="A66" s="1"/>
       <c r="B66" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>182</v>
@@ -13029,7 +13002,7 @@
     <row r="67" spans="1:54" ht="14.25" customHeight="1">
       <c r="A67" s="1"/>
       <c r="B67" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>184</v>
@@ -13146,7 +13119,7 @@
     <row r="68" spans="1:54" ht="14.25" customHeight="1">
       <c r="A68" s="1"/>
       <c r="B68" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>186</v>
@@ -13263,7 +13236,7 @@
     <row r="69" spans="1:54" ht="14.25" customHeight="1">
       <c r="A69" s="1"/>
       <c r="B69" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>188</v>
@@ -13380,7 +13353,7 @@
     <row r="70" spans="1:54" ht="14.25" customHeight="1">
       <c r="A70" s="1"/>
       <c r="B70" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>190</v>
@@ -13497,7 +13470,7 @@
     <row r="71" spans="1:54" ht="14.25" customHeight="1">
       <c r="A71" s="1"/>
       <c r="B71" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>192</v>
@@ -13614,7 +13587,7 @@
     <row r="72" spans="1:54" ht="14.25" customHeight="1">
       <c r="A72" s="1"/>
       <c r="B72" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>194</v>
@@ -13731,7 +13704,7 @@
     <row r="73" spans="1:54" ht="14.25" customHeight="1">
       <c r="A73" s="1"/>
       <c r="B73" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>196</v>
@@ -13848,7 +13821,7 @@
     <row r="74" spans="1:54" ht="14.25" customHeight="1">
       <c r="A74" s="1"/>
       <c r="B74" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>198</v>
@@ -13965,7 +13938,7 @@
     <row r="75" spans="1:54" ht="14.25" customHeight="1">
       <c r="A75" s="1"/>
       <c r="B75" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>200</v>
@@ -14082,7 +14055,7 @@
     <row r="76" spans="1:54" ht="14.25" customHeight="1">
       <c r="A76" s="1"/>
       <c r="B76" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>202</v>
@@ -14199,7 +14172,7 @@
     <row r="77" spans="1:54" ht="14.25" customHeight="1">
       <c r="A77" s="1"/>
       <c r="B77" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>204</v>
@@ -14316,7 +14289,7 @@
     <row r="78" spans="1:54" ht="14.25" customHeight="1">
       <c r="A78" s="1"/>
       <c r="B78" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>206</v>
@@ -14433,7 +14406,7 @@
     <row r="79" spans="1:54" ht="14.25" customHeight="1">
       <c r="A79" s="1"/>
       <c r="B79" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>208</v>
@@ -14550,7 +14523,7 @@
     <row r="80" spans="1:54" ht="14.25" customHeight="1">
       <c r="A80" s="1"/>
       <c r="B80" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>210</v>
@@ -14667,7 +14640,7 @@
     <row r="81" spans="1:54" ht="14.25" customHeight="1">
       <c r="A81" s="1"/>
       <c r="B81" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>212</v>
@@ -14784,7 +14757,7 @@
     <row r="82" spans="1:54" ht="14.25" customHeight="1">
       <c r="A82" s="1"/>
       <c r="B82" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>214</v>
@@ -14901,7 +14874,7 @@
     <row r="83" spans="1:54" ht="14.25" customHeight="1">
       <c r="A83" s="1"/>
       <c r="B83" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>216</v>
@@ -15018,7 +14991,7 @@
     <row r="84" spans="1:54" ht="14.25" customHeight="1">
       <c r="A84" s="1"/>
       <c r="B84" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>218</v>
@@ -15135,7 +15108,7 @@
     <row r="85" spans="1:54" ht="14.25" customHeight="1">
       <c r="A85" s="1"/>
       <c r="B85" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>220</v>
@@ -15252,7 +15225,7 @@
     <row r="86" spans="1:54" ht="14.25" customHeight="1">
       <c r="A86" s="1"/>
       <c r="B86" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>222</v>
@@ -15369,7 +15342,7 @@
     <row r="87" spans="1:54" ht="14.25" customHeight="1">
       <c r="A87" s="1"/>
       <c r="B87" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>224</v>
@@ -15485,7 +15458,7 @@
     <row r="88" spans="1:54" ht="14.25" customHeight="1">
       <c r="A88" s="1"/>
       <c r="B88" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>226</v>
@@ -15602,7 +15575,7 @@
     <row r="89" spans="1:54" ht="14.25" customHeight="1">
       <c r="A89" s="1"/>
       <c r="B89" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>228</v>
@@ -15719,7 +15692,7 @@
     <row r="90" spans="1:54" ht="14.25" customHeight="1">
       <c r="A90" s="1"/>
       <c r="B90" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>230</v>
@@ -15836,7 +15809,7 @@
     <row r="91" spans="1:54" ht="14.25" customHeight="1">
       <c r="A91" s="1"/>
       <c r="B91" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>232</v>
@@ -15953,7 +15926,7 @@
     <row r="92" spans="1:54" ht="14.25" customHeight="1">
       <c r="A92" s="1"/>
       <c r="B92" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>234</v>
@@ -16070,7 +16043,7 @@
     <row r="93" spans="1:54" ht="14.25" customHeight="1">
       <c r="A93" s="1"/>
       <c r="B93" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>236</v>
@@ -16187,7 +16160,7 @@
     <row r="94" spans="1:54" ht="14.25" customHeight="1">
       <c r="A94" s="1"/>
       <c r="B94" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>238</v>
@@ -16304,7 +16277,7 @@
     <row r="95" spans="1:54" ht="14.25" customHeight="1">
       <c r="A95" s="1"/>
       <c r="B95" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>240</v>
@@ -16421,7 +16394,7 @@
     <row r="96" spans="1:54" ht="14.25" customHeight="1">
       <c r="A96" s="1"/>
       <c r="B96" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>242</v>
@@ -16538,7 +16511,7 @@
     <row r="97" spans="1:54" ht="14.25" customHeight="1">
       <c r="A97" s="1"/>
       <c r="B97" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>244</v>
@@ -16655,7 +16628,7 @@
     <row r="98" spans="1:54" ht="14.25" customHeight="1">
       <c r="A98" s="1"/>
       <c r="B98" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>246</v>
@@ -16772,7 +16745,7 @@
     <row r="99" spans="1:54" ht="14.25" customHeight="1">
       <c r="A99" s="1"/>
       <c r="B99" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>248</v>
@@ -16889,7 +16862,7 @@
     <row r="100" spans="1:54" ht="14.25" customHeight="1">
       <c r="A100" s="1"/>
       <c r="B100" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>250</v>
@@ -17006,7 +16979,7 @@
     <row r="101" spans="1:54" ht="14.25" customHeight="1">
       <c r="A101" s="1"/>
       <c r="B101" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>252</v>
@@ -17123,7 +17096,7 @@
     <row r="102" spans="1:54" ht="14.25" customHeight="1">
       <c r="A102" s="1"/>
       <c r="B102" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>254</v>
@@ -17240,7 +17213,7 @@
     <row r="103" spans="1:54" ht="14.25" customHeight="1">
       <c r="A103" s="1"/>
       <c r="B103" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>256</v>
@@ -17357,7 +17330,7 @@
     <row r="104" spans="1:54" ht="14.25" customHeight="1">
       <c r="A104" s="1"/>
       <c r="B104" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>258</v>
@@ -17474,7 +17447,7 @@
     <row r="105" spans="1:54" ht="14.25" customHeight="1">
       <c r="A105" s="2"/>
       <c r="B105" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>260</v>
@@ -17591,7 +17564,7 @@
     <row r="106" spans="1:54" ht="14.25" customHeight="1">
       <c r="A106" s="2"/>
       <c r="B106" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>262</v>
@@ -17708,7 +17681,7 @@
     <row r="107" spans="1:54" ht="14.25" customHeight="1">
       <c r="A107" s="1"/>
       <c r="B107" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>264</v>
@@ -17825,7 +17798,7 @@
     <row r="108" spans="1:54" ht="14.25" customHeight="1">
       <c r="A108" s="1"/>
       <c r="B108" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>266</v>
@@ -17942,7 +17915,7 @@
     <row r="109" spans="1:54" ht="14.25" customHeight="1">
       <c r="A109" s="1"/>
       <c r="B109" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>268</v>
@@ -18059,7 +18032,7 @@
     <row r="110" spans="1:54" ht="14.25" customHeight="1">
       <c r="A110" s="1"/>
       <c r="B110" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>270</v>
@@ -18176,7 +18149,7 @@
     <row r="111" spans="1:54" ht="14.25" customHeight="1">
       <c r="A111" s="1"/>
       <c r="B111" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>272</v>
@@ -18293,7 +18266,7 @@
     <row r="112" spans="1:54" ht="14.25" customHeight="1">
       <c r="A112" s="1"/>
       <c r="B112" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>274</v>
@@ -18410,7 +18383,7 @@
     <row r="113" spans="1:54" ht="14.25" customHeight="1">
       <c r="A113" s="1"/>
       <c r="B113" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>276</v>
@@ -18527,7 +18500,7 @@
     <row r="114" spans="1:54" ht="14.25" customHeight="1">
       <c r="A114" s="1"/>
       <c r="B114" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>278</v>
@@ -18644,7 +18617,7 @@
     <row r="115" spans="1:54" ht="14.25" customHeight="1">
       <c r="A115" s="1"/>
       <c r="B115" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>280</v>
@@ -18761,7 +18734,7 @@
     <row r="116" spans="1:54" ht="14.25" customHeight="1">
       <c r="A116" s="1"/>
       <c r="B116" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>282</v>
@@ -18878,7 +18851,7 @@
     <row r="117" spans="1:54" ht="14.25" customHeight="1">
       <c r="A117" s="1"/>
       <c r="B117" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>284</v>
@@ -18995,7 +18968,7 @@
     <row r="118" spans="1:54" ht="14.25" customHeight="1">
       <c r="A118" s="1"/>
       <c r="B118" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>286</v>
@@ -19112,7 +19085,7 @@
     <row r="119" spans="1:54" ht="14.25" customHeight="1">
       <c r="A119" s="1"/>
       <c r="B119" s="46" t="s">
-        <v>1359</v>
+        <v>38</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>288</v>
@@ -19283,7 +19256,7 @@
         <v>290</v>
       </c>
       <c r="B121" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>291</v>
@@ -19404,7 +19377,7 @@
         <v>296</v>
       </c>
       <c r="B122" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>297</v>
@@ -19525,7 +19498,7 @@
         <v>51</v>
       </c>
       <c r="B123" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>301</v>
@@ -19645,7 +19618,7 @@
         <v>51</v>
       </c>
       <c r="B124" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>304</v>
@@ -19766,7 +19739,7 @@
         <v>51</v>
       </c>
       <c r="B125" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>307</v>
@@ -19886,7 +19859,7 @@
         <v>51</v>
       </c>
       <c r="B126" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>311</v>
@@ -20007,7 +19980,7 @@
         <v>51</v>
       </c>
       <c r="B127" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>315</v>
@@ -20128,7 +20101,7 @@
         <v>51</v>
       </c>
       <c r="B128" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>319</v>
@@ -20248,7 +20221,7 @@
         <v>51</v>
       </c>
       <c r="B129" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>323</v>
@@ -20369,7 +20342,7 @@
         <v>51</v>
       </c>
       <c r="B130" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>326</v>
@@ -20490,7 +20463,7 @@
         <v>51</v>
       </c>
       <c r="B131" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>329</v>
@@ -20609,7 +20582,7 @@
     <row r="132" spans="1:54" ht="14.25" customHeight="1">
       <c r="A132" s="1"/>
       <c r="B132" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>332</v>
@@ -20730,7 +20703,7 @@
         <v>51</v>
       </c>
       <c r="B133" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>335</v>
@@ -20851,7 +20824,7 @@
         <v>51</v>
       </c>
       <c r="B134" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>338</v>
@@ -20971,7 +20944,7 @@
     <row r="135" spans="1:54" ht="14.25" customHeight="1">
       <c r="A135" s="2"/>
       <c r="B135" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>341</v>
@@ -21088,7 +21061,7 @@
     <row r="136" spans="1:54" ht="14.25" customHeight="1">
       <c r="A136" s="1"/>
       <c r="B136" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>343</v>
@@ -21207,7 +21180,7 @@
         <v>51</v>
       </c>
       <c r="B137" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>345</v>
@@ -21327,7 +21300,7 @@
         <v>51</v>
       </c>
       <c r="B138" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>348</v>
@@ -21448,7 +21421,7 @@
         <v>51</v>
       </c>
       <c r="B139" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>351</v>
@@ -21569,7 +21542,7 @@
         <v>51</v>
       </c>
       <c r="B140" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>354</v>
@@ -21690,7 +21663,7 @@
         <v>51</v>
       </c>
       <c r="B141" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>357</v>
@@ -21812,7 +21785,7 @@
         <v>51</v>
       </c>
       <c r="B142" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>360</v>
@@ -21931,7 +21904,7 @@
     <row r="143" spans="1:54" ht="14.25" customHeight="1">
       <c r="A143" s="1"/>
       <c r="B143" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C143" s="3" t="s">
         <v>363</v>
@@ -22050,7 +22023,7 @@
         <v>51</v>
       </c>
       <c r="B144" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>365</v>
@@ -22171,7 +22144,7 @@
         <v>51</v>
       </c>
       <c r="B145" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>369</v>
@@ -22292,7 +22265,7 @@
         <v>51</v>
       </c>
       <c r="B146" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>373</v>
@@ -22413,7 +22386,7 @@
         <v>51</v>
       </c>
       <c r="B147" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C147" s="2" t="s">
         <v>376</v>
@@ -22534,7 +22507,7 @@
         <v>51</v>
       </c>
       <c r="B148" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>379</v>
@@ -22655,7 +22628,7 @@
         <v>51</v>
       </c>
       <c r="B149" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>382</v>
@@ -22776,7 +22749,7 @@
         <v>51</v>
       </c>
       <c r="B150" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>386</v>
@@ -22897,7 +22870,7 @@
         <v>51</v>
       </c>
       <c r="B151" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>390</v>
@@ -23019,7 +22992,7 @@
         <v>51</v>
       </c>
       <c r="B152" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>394</v>
@@ -23140,7 +23113,7 @@
         <v>51</v>
       </c>
       <c r="B153" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C153" s="2" t="s">
         <v>397</v>
@@ -23261,7 +23234,7 @@
         <v>51</v>
       </c>
       <c r="B154" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>401</v>
@@ -23382,7 +23355,7 @@
         <v>51</v>
       </c>
       <c r="B155" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>403</v>
@@ -23503,7 +23476,7 @@
         <v>51</v>
       </c>
       <c r="B156" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>405</v>
@@ -23624,7 +23597,7 @@
         <v>51</v>
       </c>
       <c r="B157" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>407</v>
@@ -23745,7 +23718,7 @@
         <v>51</v>
       </c>
       <c r="B158" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>409</v>
@@ -23866,7 +23839,7 @@
         <v>51</v>
       </c>
       <c r="B159" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>412</v>
@@ -23987,7 +23960,7 @@
         <v>51</v>
       </c>
       <c r="B160" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>415</v>
@@ -24108,7 +24081,7 @@
         <v>51</v>
       </c>
       <c r="B161" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>419</v>
@@ -24229,7 +24202,7 @@
         <v>51</v>
       </c>
       <c r="B162" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>422</v>
@@ -24350,7 +24323,7 @@
         <v>425</v>
       </c>
       <c r="B163" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
@@ -24461,7 +24434,7 @@
         <v>425</v>
       </c>
       <c r="B164" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
@@ -24571,7 +24544,7 @@
         <v>425</v>
       </c>
       <c r="B165" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C165" s="2"/>
       <c r="D165" s="2"/>
@@ -24682,7 +24655,7 @@
         <v>425</v>
       </c>
       <c r="B166" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C166" s="2"/>
       <c r="D166" s="2"/>
@@ -24793,7 +24766,7 @@
         <v>425</v>
       </c>
       <c r="B167" s="46" t="s">
-        <v>1360</v>
+        <v>296</v>
       </c>
       <c r="C167" s="2"/>
       <c r="D167" s="2"/>
@@ -24957,7 +24930,7 @@
         <v>435</v>
       </c>
       <c r="B169" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>436</v>
@@ -25078,7 +25051,7 @@
         <v>440</v>
       </c>
       <c r="B170" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>441</v>
@@ -25197,7 +25170,7 @@
     <row r="171" spans="1:54" ht="14.25" customHeight="1">
       <c r="A171" s="1"/>
       <c r="B171" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>444</v>
@@ -25316,7 +25289,7 @@
     <row r="172" spans="1:54" ht="14.25" customHeight="1">
       <c r="A172" s="1"/>
       <c r="B172" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>447</v>
@@ -25438,7 +25411,7 @@
         <v>51</v>
       </c>
       <c r="B173" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>451</v>
@@ -25559,7 +25532,7 @@
         <v>51</v>
       </c>
       <c r="B174" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>455</v>
@@ -25680,7 +25653,7 @@
         <v>51</v>
       </c>
       <c r="B175" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>458</v>
@@ -25801,7 +25774,7 @@
         <v>51</v>
       </c>
       <c r="B176" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>461</v>
@@ -25922,7 +25895,7 @@
         <v>51</v>
       </c>
       <c r="B177" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>464</v>
@@ -26044,7 +26017,7 @@
         <v>51</v>
       </c>
       <c r="B178" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C178" s="2" t="s">
         <v>466</v>
@@ -26165,7 +26138,7 @@
         <v>51</v>
       </c>
       <c r="B179" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C179" s="2" t="s">
         <v>468</v>
@@ -26287,7 +26260,7 @@
         <v>51</v>
       </c>
       <c r="B180" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C180" s="2" t="s">
         <v>471</v>
@@ -26408,7 +26381,7 @@
         <v>51</v>
       </c>
       <c r="B181" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C181" s="2" t="s">
         <v>474</v>
@@ -26530,7 +26503,7 @@
         <v>51</v>
       </c>
       <c r="B182" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>477</v>
@@ -26651,7 +26624,7 @@
         <v>51</v>
       </c>
       <c r="B183" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C183" s="2" t="s">
         <v>481</v>
@@ -26772,7 +26745,7 @@
         <v>51</v>
       </c>
       <c r="B184" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>485</v>
@@ -26893,7 +26866,7 @@
         <v>51</v>
       </c>
       <c r="B185" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>488</v>
@@ -27014,7 +26987,7 @@
         <v>51</v>
       </c>
       <c r="B186" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>491</v>
@@ -27135,7 +27108,7 @@
         <v>51</v>
       </c>
       <c r="B187" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>494</v>
@@ -27256,7 +27229,7 @@
         <v>51</v>
       </c>
       <c r="B188" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>497</v>
@@ -27377,7 +27350,7 @@
         <v>51</v>
       </c>
       <c r="B189" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>500</v>
@@ -27498,7 +27471,7 @@
         <v>51</v>
       </c>
       <c r="B190" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C190" s="2" t="s">
         <v>503</v>
@@ -27619,7 +27592,7 @@
         <v>51</v>
       </c>
       <c r="B191" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C191" s="2" t="s">
         <v>505</v>
@@ -27740,7 +27713,7 @@
         <v>51</v>
       </c>
       <c r="B192" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C192" s="2" t="s">
         <v>508</v>
@@ -27861,7 +27834,7 @@
         <v>51</v>
       </c>
       <c r="B193" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C193" s="2" t="s">
         <v>511</v>
@@ -27982,7 +27955,7 @@
         <v>51</v>
       </c>
       <c r="B194" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C194" s="2" t="s">
         <v>513</v>
@@ -28101,7 +28074,7 @@
     <row r="195" spans="1:54" ht="14.25" customHeight="1">
       <c r="A195" s="1"/>
       <c r="B195" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C195" s="2" t="s">
         <v>516</v>
@@ -28222,7 +28195,7 @@
         <v>519</v>
       </c>
       <c r="B196" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C196" s="2" t="s">
         <v>520</v>
@@ -28339,7 +28312,7 @@
     <row r="197" spans="1:54" ht="14.25" customHeight="1">
       <c r="A197" s="2"/>
       <c r="B197" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>522</v>
@@ -28456,7 +28429,7 @@
     <row r="198" spans="1:54" ht="14.25" customHeight="1">
       <c r="A198" s="2"/>
       <c r="B198" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>524</v>
@@ -28573,7 +28546,7 @@
     <row r="199" spans="1:54" ht="14.25" customHeight="1">
       <c r="A199" s="2"/>
       <c r="B199" s="46" t="s">
-        <v>1361</v>
+        <v>440</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>526</v>
@@ -28743,7 +28716,7 @@
         <v>528</v>
       </c>
       <c r="B201" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>529</v>
@@ -28864,7 +28837,7 @@
         <v>532</v>
       </c>
       <c r="B202" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C202" s="2" t="s">
         <v>533</v>
@@ -28982,7 +28955,7 @@
     <row r="203" spans="1:54" ht="14.25" customHeight="1">
       <c r="A203" s="1"/>
       <c r="B203" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C203" s="2" t="s">
         <v>536</v>
@@ -29101,7 +29074,7 @@
     <row r="204" spans="1:54" ht="14.25" customHeight="1">
       <c r="A204" s="1"/>
       <c r="B204" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C204" s="2" t="s">
         <v>538</v>
@@ -29220,7 +29193,7 @@
     <row r="205" spans="1:54" ht="14.25" customHeight="1">
       <c r="A205" s="1"/>
       <c r="B205" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>542</v>
@@ -29339,7 +29312,7 @@
     <row r="206" spans="1:54" ht="14.25" customHeight="1">
       <c r="A206" s="1"/>
       <c r="B206" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>544</v>
@@ -29460,7 +29433,7 @@
         <v>51</v>
       </c>
       <c r="B207" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C207" s="2" t="s">
         <v>548</v>
@@ -29579,7 +29552,7 @@
         <v>51</v>
       </c>
       <c r="B208" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C208" s="2" t="s">
         <v>550</v>
@@ -29698,7 +29671,7 @@
     <row r="209" spans="1:54" ht="14.25" customHeight="1">
       <c r="A209" s="1"/>
       <c r="B209" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C209" s="2" t="s">
         <v>552</v>
@@ -29819,7 +29792,7 @@
         <v>51</v>
       </c>
       <c r="B210" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C210" s="2" t="s">
         <v>554</v>
@@ -29940,7 +29913,7 @@
         <v>51</v>
       </c>
       <c r="B211" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C211" s="2" t="s">
         <v>556</v>
@@ -30061,7 +30034,7 @@
         <v>51</v>
       </c>
       <c r="B212" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C212" s="2" t="s">
         <v>558</v>
@@ -30179,7 +30152,7 @@
     <row r="213" spans="1:54" ht="14.25" customHeight="1">
       <c r="A213" s="2"/>
       <c r="B213" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C213" s="2" t="s">
         <v>560</v>
@@ -30296,7 +30269,7 @@
     <row r="214" spans="1:54" ht="14.25" customHeight="1">
       <c r="A214" s="2"/>
       <c r="B214" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C214" s="2" t="s">
         <v>563</v>
@@ -30412,7 +30385,7 @@
     <row r="215" spans="1:54" ht="14.25" customHeight="1">
       <c r="A215" s="1"/>
       <c r="B215" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C215" s="3" t="s">
         <v>565</v>
@@ -30529,7 +30502,7 @@
     <row r="216" spans="1:54" ht="14.25" customHeight="1">
       <c r="A216" s="1"/>
       <c r="B216" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C216" s="3" t="s">
         <v>567</v>
@@ -30646,7 +30619,7 @@
     <row r="217" spans="1:54" ht="14.25" customHeight="1">
       <c r="A217" s="1"/>
       <c r="B217" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C217" s="3" t="s">
         <v>569</v>
@@ -30763,7 +30736,7 @@
     <row r="218" spans="1:54" ht="14.25" customHeight="1">
       <c r="A218" s="1"/>
       <c r="B218" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C218" s="3" t="s">
         <v>571</v>
@@ -30882,7 +30855,7 @@
         <v>51</v>
       </c>
       <c r="B219" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>573</v>
@@ -31001,7 +30974,7 @@
     <row r="220" spans="1:54" ht="14.25" customHeight="1">
       <c r="A220" s="1"/>
       <c r="B220" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C220" s="3" t="s">
         <v>576</v>
@@ -31118,7 +31091,7 @@
     <row r="221" spans="1:54" ht="14.25" customHeight="1">
       <c r="A221" s="1"/>
       <c r="B221" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C221" s="3" t="s">
         <v>578</v>
@@ -31235,7 +31208,7 @@
     <row r="222" spans="1:54" ht="14.25" customHeight="1">
       <c r="A222" s="1"/>
       <c r="B222" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C222" s="3" t="s">
         <v>580</v>
@@ -31352,7 +31325,7 @@
     <row r="223" spans="1:54" ht="14.25" customHeight="1">
       <c r="A223" s="1"/>
       <c r="B223" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>582</v>
@@ -31469,7 +31442,7 @@
     <row r="224" spans="1:54" ht="14.25" customHeight="1">
       <c r="A224" s="1"/>
       <c r="B224" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C224" s="3" t="s">
         <v>584</v>
@@ -31586,7 +31559,7 @@
     <row r="225" spans="1:41" ht="14.25" customHeight="1">
       <c r="A225" s="1"/>
       <c r="B225" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C225" s="3" t="s">
         <v>586</v>
@@ -31697,7 +31670,7 @@
     <row r="226" spans="1:41" ht="14.25" customHeight="1">
       <c r="A226" s="1"/>
       <c r="B226" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C226" s="3" t="s">
         <v>588</v>
@@ -31808,7 +31781,7 @@
     <row r="227" spans="1:41" ht="14.25" customHeight="1">
       <c r="A227" s="1"/>
       <c r="B227" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C227" s="3" t="s">
         <v>590</v>
@@ -31919,7 +31892,7 @@
     <row r="228" spans="1:41" ht="14.25" customHeight="1">
       <c r="A228" s="1"/>
       <c r="B228" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C228" s="3" t="s">
         <v>592</v>
@@ -32030,7 +32003,7 @@
     <row r="229" spans="1:41" ht="14.25" customHeight="1">
       <c r="A229" s="1"/>
       <c r="B229" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C229" s="3" t="s">
         <v>594</v>
@@ -32140,7 +32113,7 @@
     <row r="230" spans="1:41" ht="14.25" customHeight="1">
       <c r="A230" s="1"/>
       <c r="B230" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C230" s="2" t="s">
         <v>596</v>
@@ -32250,7 +32223,7 @@
     <row r="231" spans="1:41" ht="14.25" customHeight="1">
       <c r="A231" s="1"/>
       <c r="B231" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>598</v>
@@ -32363,7 +32336,7 @@
         <v>51</v>
       </c>
       <c r="B232" s="46" t="s">
-        <v>1362</v>
+        <v>532</v>
       </c>
       <c r="C232" s="2" t="s">
         <v>600</v>
@@ -32524,7 +32497,7 @@
         <v>602</v>
       </c>
       <c r="B234" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C234" s="2" t="s">
         <v>603</v>
@@ -32639,7 +32612,7 @@
         <v>606</v>
       </c>
       <c r="B235" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C235" s="2" t="s">
         <v>607</v>
@@ -32754,7 +32727,7 @@
         <v>51</v>
       </c>
       <c r="B236" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C236" s="2" t="s">
         <v>610</v>
@@ -32867,7 +32840,7 @@
     <row r="237" spans="1:41" ht="14.25" customHeight="1">
       <c r="A237" s="1"/>
       <c r="B237" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C237" s="2" t="s">
         <v>614</v>
@@ -32982,7 +32955,7 @@
         <v>51</v>
       </c>
       <c r="B238" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C238" s="2" t="s">
         <v>617</v>
@@ -33097,7 +33070,7 @@
         <v>51</v>
       </c>
       <c r="B239" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C239" s="2" t="s">
         <v>620</v>
@@ -33212,7 +33185,7 @@
         <v>51</v>
       </c>
       <c r="B240" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C240" s="2" t="s">
         <v>622</v>
@@ -33327,7 +33300,7 @@
         <v>51</v>
       </c>
       <c r="B241" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C241" s="2" t="s">
         <v>625</v>
@@ -33442,7 +33415,7 @@
         <v>51</v>
       </c>
       <c r="B242" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C242" s="2" t="s">
         <v>627</v>
@@ -33557,7 +33530,7 @@
         <v>51</v>
       </c>
       <c r="B243" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C243" s="2" t="s">
         <v>629</v>
@@ -33672,7 +33645,7 @@
         <v>51</v>
       </c>
       <c r="B244" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C244" s="2" t="s">
         <v>631</v>
@@ -33787,7 +33760,7 @@
         <v>51</v>
       </c>
       <c r="B245" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C245" s="2" t="s">
         <v>633</v>
@@ -33902,7 +33875,7 @@
         <v>51</v>
       </c>
       <c r="B246" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C246" s="2" t="s">
         <v>635</v>
@@ -34017,7 +33990,7 @@
         <v>51</v>
       </c>
       <c r="B247" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C247" s="2" t="s">
         <v>637</v>
@@ -34132,7 +34105,7 @@
         <v>51</v>
       </c>
       <c r="B248" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C248" s="2" t="s">
         <v>639</v>
@@ -34247,7 +34220,7 @@
         <v>51</v>
       </c>
       <c r="B249" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C249" s="2" t="s">
         <v>641</v>
@@ -34362,7 +34335,7 @@
         <v>51</v>
       </c>
       <c r="B250" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C250" s="2" t="s">
         <v>644</v>
@@ -34477,7 +34450,7 @@
         <v>51</v>
       </c>
       <c r="B251" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C251" s="2" t="s">
         <v>646</v>
@@ -34592,7 +34565,7 @@
         <v>51</v>
       </c>
       <c r="B252" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C252" s="2" t="s">
         <v>648</v>
@@ -34707,7 +34680,7 @@
         <v>650</v>
       </c>
       <c r="B253" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C253" s="2" t="s">
         <v>651</v>
@@ -34818,7 +34791,7 @@
     <row r="254" spans="1:41" ht="14.25" customHeight="1">
       <c r="A254" s="2"/>
       <c r="B254" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C254" s="2" t="s">
         <v>653</v>
@@ -34929,7 +34902,7 @@
     <row r="255" spans="1:41" ht="14.25" customHeight="1">
       <c r="A255" s="7"/>
       <c r="B255" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C255" s="2" t="s">
         <v>655</v>
@@ -35042,7 +35015,7 @@
         <v>657</v>
       </c>
       <c r="B256" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C256" s="2" t="s">
         <v>658</v>
@@ -35153,7 +35126,7 @@
     <row r="257" spans="1:41" ht="14.25" customHeight="1">
       <c r="A257" s="7"/>
       <c r="B257" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C257" s="2" t="s">
         <v>661</v>
@@ -35264,7 +35237,7 @@
     <row r="258" spans="1:41" ht="14.25" customHeight="1">
       <c r="A258" s="63"/>
       <c r="B258" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C258" s="2" t="s">
         <v>663</v>
@@ -35375,7 +35348,7 @@
     <row r="259" spans="1:41" ht="14.25" customHeight="1">
       <c r="A259" s="2"/>
       <c r="B259" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C259" s="2" t="s">
         <v>665</v>
@@ -35486,7 +35459,7 @@
     <row r="260" spans="1:41" ht="14.25" customHeight="1">
       <c r="A260" s="2"/>
       <c r="B260" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C260" s="2" t="s">
         <v>667</v>
@@ -35599,7 +35572,7 @@
         <v>519</v>
       </c>
       <c r="B261" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C261" s="2" t="s">
         <v>670</v>
@@ -35709,7 +35682,7 @@
     <row r="262" spans="1:41" ht="14.25" customHeight="1">
       <c r="A262" s="2"/>
       <c r="B262" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C262" s="2" t="s">
         <v>672</v>
@@ -35820,7 +35793,7 @@
     <row r="263" spans="1:41" ht="14.25" customHeight="1">
       <c r="A263" s="2"/>
       <c r="B263" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C263" s="2" t="s">
         <v>674</v>
@@ -35931,7 +35904,7 @@
     <row r="264" spans="1:41" ht="14.25" customHeight="1">
       <c r="A264" s="2"/>
       <c r="B264" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C264" s="2" t="s">
         <v>676</v>
@@ -36042,7 +36015,7 @@
     <row r="265" spans="1:41" ht="14.25" customHeight="1">
       <c r="A265" s="2"/>
       <c r="B265" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C265" s="2" t="s">
         <v>678</v>
@@ -36153,7 +36126,7 @@
     <row r="266" spans="1:41" ht="14.25" customHeight="1">
       <c r="A266" s="2"/>
       <c r="B266" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C266" s="2" t="s">
         <v>680</v>
@@ -36264,7 +36237,7 @@
     <row r="267" spans="1:41" ht="14.25" customHeight="1">
       <c r="A267" s="1"/>
       <c r="B267" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C267" s="2" t="s">
         <v>682</v>
@@ -36375,7 +36348,7 @@
     <row r="268" spans="1:41" ht="14.25" customHeight="1">
       <c r="A268" s="1"/>
       <c r="B268" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C268" s="2" t="s">
         <v>684</v>
@@ -36486,7 +36459,7 @@
     <row r="269" spans="1:41" ht="14.25" customHeight="1">
       <c r="A269" s="1"/>
       <c r="B269" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C269" s="2" t="s">
         <v>686</v>
@@ -36601,7 +36574,7 @@
         <v>51</v>
       </c>
       <c r="B270" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C270" s="2" t="s">
         <v>688</v>
@@ -36713,7 +36686,7 @@
     <row r="271" spans="1:41" ht="14.25" customHeight="1">
       <c r="A271" s="2"/>
       <c r="B271" s="46" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="C271" s="2" t="s">
         <v>690</v>
@@ -36872,7 +36845,7 @@
         <v>692</v>
       </c>
       <c r="B273" s="46" t="s">
-        <v>1364</v>
+        <v>695</v>
       </c>
       <c r="C273" s="2" t="s">
         <v>693</v>
@@ -36985,7 +36958,7 @@
         <v>695</v>
       </c>
       <c r="B274" s="46" t="s">
-        <v>1364</v>
+        <v>695</v>
       </c>
       <c r="C274" s="2" t="s">
         <v>696</v>
@@ -37095,7 +37068,7 @@
     <row r="275" spans="1:41" ht="14.25" customHeight="1">
       <c r="A275" s="1"/>
       <c r="B275" s="46" t="s">
-        <v>1364</v>
+        <v>695</v>
       </c>
       <c r="C275" s="2" t="s">
         <v>698</v>
@@ -37210,7 +37183,7 @@
         <v>51</v>
       </c>
       <c r="B276" s="46" t="s">
-        <v>1364</v>
+        <v>695</v>
       </c>
       <c r="C276" s="2" t="s">
         <v>702</v>
@@ -37325,7 +37298,7 @@
         <v>51</v>
       </c>
       <c r="B277" s="46" t="s">
-        <v>1364</v>
+        <v>695</v>
       </c>
       <c r="C277" s="2" t="s">
         <v>704</v>
@@ -37438,7 +37411,7 @@
     <row r="278" spans="1:41" ht="14.25" customHeight="1">
       <c r="A278" s="1"/>
       <c r="B278" s="46" t="s">
-        <v>1364</v>
+        <v>695</v>
       </c>
       <c r="C278" s="2" t="s">
         <v>706</v>
@@ -37549,7 +37522,7 @@
     <row r="279" spans="1:41" ht="14.25" customHeight="1">
       <c r="A279" s="1"/>
       <c r="B279" s="46" t="s">
-        <v>1364</v>
+        <v>695</v>
       </c>
       <c r="C279" s="2" t="s">
         <v>708</v>
@@ -37660,7 +37633,7 @@
     <row r="280" spans="1:41" ht="14.25" customHeight="1">
       <c r="A280" s="1"/>
       <c r="B280" s="46" t="s">
-        <v>1364</v>
+        <v>695</v>
       </c>
       <c r="C280" s="2" t="s">
         <v>710</v>
@@ -37771,7 +37744,7 @@
     <row r="281" spans="1:41" ht="14.25" customHeight="1">
       <c r="A281" s="2"/>
       <c r="B281" s="46" t="s">
-        <v>1364</v>
+        <v>695</v>
       </c>
       <c r="C281" s="2" t="s">
         <v>712</v>
@@ -37882,7 +37855,7 @@
     <row r="282" spans="1:41" ht="14.25" customHeight="1">
       <c r="A282" s="1"/>
       <c r="B282" s="46" t="s">
-        <v>1364</v>
+        <v>695</v>
       </c>
       <c r="C282" s="2" t="s">
         <v>714</v>
@@ -37993,7 +37966,7 @@
     <row r="283" spans="1:41" ht="14.25" customHeight="1">
       <c r="A283" s="1"/>
       <c r="B283" s="46" t="s">
-        <v>1364</v>
+        <v>695</v>
       </c>
       <c r="C283" s="2" t="s">
         <v>716</v>
@@ -38152,7 +38125,7 @@
         <v>718</v>
       </c>
       <c r="B285" s="46" t="s">
-        <v>1365</v>
+        <v>722</v>
       </c>
       <c r="C285" s="2" t="s">
         <v>719</v>
@@ -38265,7 +38238,7 @@
         <v>722</v>
       </c>
       <c r="B286" s="46" t="s">
-        <v>1365</v>
+        <v>722</v>
       </c>
       <c r="C286" s="2" t="s">
         <v>723</v>
@@ -38380,7 +38353,7 @@
         <v>51</v>
       </c>
       <c r="B287" s="46" t="s">
-        <v>1365</v>
+        <v>722</v>
       </c>
       <c r="C287" s="2" t="s">
         <v>726</v>
@@ -38493,7 +38466,7 @@
     <row r="288" spans="1:41" ht="14.25" customHeight="1">
       <c r="A288" s="1"/>
       <c r="B288" s="46" t="s">
-        <v>1365</v>
+        <v>722</v>
       </c>
       <c r="C288" s="2" t="s">
         <v>676</v>
@@ -38608,7 +38581,7 @@
         <v>51</v>
       </c>
       <c r="B289" s="46" t="s">
-        <v>1365</v>
+        <v>722</v>
       </c>
       <c r="C289" s="2" t="s">
         <v>731</v>
@@ -38723,7 +38696,7 @@
         <v>51</v>
       </c>
       <c r="B290" s="46" t="s">
-        <v>1365</v>
+        <v>722</v>
       </c>
       <c r="C290" s="2" t="s">
         <v>734</v>
@@ -38838,7 +38811,7 @@
         <v>51</v>
       </c>
       <c r="B291" s="46" t="s">
-        <v>1365</v>
+        <v>722</v>
       </c>
       <c r="C291" s="2" t="s">
         <v>737</v>
@@ -38953,7 +38926,7 @@
         <v>51</v>
       </c>
       <c r="B292" s="46" t="s">
-        <v>1365</v>
+        <v>722</v>
       </c>
       <c r="C292" s="2" t="s">
         <v>739</v>
@@ -39068,7 +39041,7 @@
         <v>51</v>
       </c>
       <c r="B293" s="46" t="s">
-        <v>1365</v>
+        <v>722</v>
       </c>
       <c r="C293" s="2" t="s">
         <v>742</v>
@@ -39183,7 +39156,7 @@
         <v>51</v>
       </c>
       <c r="B294" s="46" t="s">
-        <v>1365</v>
+        <v>722</v>
       </c>
       <c r="C294" s="2" t="s">
         <v>745</v>
@@ -39298,7 +39271,7 @@
         <v>51</v>
       </c>
       <c r="B295" s="46" t="s">
-        <v>1365</v>
+        <v>722</v>
       </c>
       <c r="C295" s="2" t="s">
         <v>747</v>
@@ -39413,7 +39386,7 @@
         <v>51</v>
       </c>
       <c r="B296" s="46" t="s">
-        <v>1365</v>
+        <v>722</v>
       </c>
       <c r="C296" s="2" t="s">
         <v>749</v>
@@ -39526,7 +39499,7 @@
         <v>51</v>
       </c>
       <c r="B297" s="46" t="s">
-        <v>1365</v>
+        <v>722</v>
       </c>
       <c r="C297" s="2" t="s">
         <v>751</v>
@@ -39636,7 +39609,7 @@
     <row r="298" spans="1:41" ht="14.25" customHeight="1">
       <c r="A298" s="2"/>
       <c r="B298" s="46" t="s">
-        <v>1365</v>
+        <v>722</v>
       </c>
       <c r="C298" s="2" t="s">
         <v>753</v>
@@ -39797,7 +39770,7 @@
         <v>755</v>
       </c>
       <c r="B300" s="46" t="s">
-        <v>1366</v>
+        <v>759</v>
       </c>
       <c r="C300" s="2" t="s">
         <v>756</v>
@@ -39917,7 +39890,7 @@
         <v>759</v>
       </c>
       <c r="B301" s="46" t="s">
-        <v>1366</v>
+        <v>759</v>
       </c>
       <c r="C301" s="2" t="s">
         <v>760</v>
@@ -40036,7 +40009,7 @@
         <v>51</v>
       </c>
       <c r="B302" s="46" t="s">
-        <v>1366</v>
+        <v>759</v>
       </c>
       <c r="C302" s="2" t="s">
         <v>762</v>
@@ -40156,7 +40129,7 @@
         <v>51</v>
       </c>
       <c r="B303" s="46" t="s">
-        <v>1366</v>
+        <v>759</v>
       </c>
       <c r="C303" s="2" t="s">
         <v>764</v>
@@ -40277,7 +40250,7 @@
         <v>51</v>
       </c>
       <c r="B304" s="46" t="s">
-        <v>1366</v>
+        <v>759</v>
       </c>
       <c r="C304" s="2" t="s">
         <v>766</v>
@@ -40397,7 +40370,7 @@
         <v>51</v>
       </c>
       <c r="B305" s="46" t="s">
-        <v>1366</v>
+        <v>759</v>
       </c>
       <c r="C305" s="2" t="s">
         <v>769</v>
@@ -40512,7 +40485,7 @@
         <v>51</v>
       </c>
       <c r="B306" s="46" t="s">
-        <v>1366</v>
+        <v>759</v>
       </c>
       <c r="C306" s="2" t="s">
         <v>771</v>
@@ -40627,7 +40600,7 @@
         <v>51</v>
       </c>
       <c r="B307" s="46" t="s">
-        <v>1366</v>
+        <v>759</v>
       </c>
       <c r="C307" s="2" t="s">
         <v>773</v>
@@ -40742,7 +40715,7 @@
         <v>51</v>
       </c>
       <c r="B308" s="46" t="s">
-        <v>1366</v>
+        <v>759</v>
       </c>
       <c r="C308" s="2" t="s">
         <v>775</v>
@@ -40857,7 +40830,7 @@
         <v>51</v>
       </c>
       <c r="B309" s="46" t="s">
-        <v>1366</v>
+        <v>759</v>
       </c>
       <c r="C309" s="2" t="s">
         <v>777</v>
@@ -40972,7 +40945,7 @@
         <v>51</v>
       </c>
       <c r="B310" s="46" t="s">
-        <v>1366</v>
+        <v>759</v>
       </c>
       <c r="C310" s="2" t="s">
         <v>779</v>
@@ -41087,7 +41060,7 @@
         <v>51</v>
       </c>
       <c r="B311" s="46" t="s">
-        <v>1366</v>
+        <v>759</v>
       </c>
       <c r="C311" s="2" t="s">
         <v>781</v>
@@ -41200,7 +41173,7 @@
     <row r="312" spans="1:41" ht="14.25" customHeight="1">
       <c r="A312" s="1"/>
       <c r="B312" s="46" t="s">
-        <v>1366</v>
+        <v>759</v>
       </c>
       <c r="C312" s="2" t="s">
         <v>783</v>
@@ -41361,7 +41334,7 @@
         <v>785</v>
       </c>
       <c r="B314" s="46" t="s">
-        <v>1367</v>
+        <v>788</v>
       </c>
       <c r="C314" s="2" t="s">
         <v>786</v>
@@ -41476,7 +41449,7 @@
         <v>788</v>
       </c>
       <c r="B315" s="46" t="s">
-        <v>1367</v>
+        <v>788</v>
       </c>
       <c r="C315" s="2" t="s">
         <v>789</v>
@@ -41589,7 +41562,7 @@
     <row r="316" spans="1:41" ht="14.25" customHeight="1">
       <c r="A316" s="1"/>
       <c r="B316" s="46" t="s">
-        <v>1367</v>
+        <v>788</v>
       </c>
       <c r="C316" s="2" t="s">
         <v>792</v>
@@ -41704,7 +41677,7 @@
         <v>51</v>
       </c>
       <c r="B317" s="46" t="s">
-        <v>1367</v>
+        <v>788</v>
       </c>
       <c r="C317" s="2" t="s">
         <v>794</v>
@@ -41819,7 +41792,7 @@
         <v>51</v>
       </c>
       <c r="B318" s="46" t="s">
-        <v>1367</v>
+        <v>788</v>
       </c>
       <c r="C318" s="2" t="s">
         <v>796</v>
@@ -41932,7 +41905,7 @@
         <v>51</v>
       </c>
       <c r="B319" s="46" t="s">
-        <v>1367</v>
+        <v>788</v>
       </c>
       <c r="C319" s="2" t="s">
         <v>799</v>
@@ -42047,7 +42020,7 @@
         <v>801</v>
       </c>
       <c r="B320" s="46" t="s">
-        <v>1367</v>
+        <v>788</v>
       </c>
       <c r="C320" s="2"/>
       <c r="D320" s="2"/>
@@ -42151,7 +42124,7 @@
         <v>51</v>
       </c>
       <c r="B321" s="46" t="s">
-        <v>1367</v>
+        <v>788</v>
       </c>
       <c r="C321" s="2"/>
       <c r="D321" s="2"/>
@@ -42254,7 +42227,7 @@
     <row r="322" spans="1:41" ht="14.25" customHeight="1">
       <c r="A322" s="1"/>
       <c r="B322" s="46" t="s">
-        <v>1367</v>
+        <v>788</v>
       </c>
       <c r="C322" s="2"/>
       <c r="D322" s="2"/>
@@ -42357,7 +42330,7 @@
     <row r="323" spans="1:41" ht="14.25" customHeight="1">
       <c r="A323" s="1"/>
       <c r="B323" s="46" t="s">
-        <v>1367</v>
+        <v>788</v>
       </c>
       <c r="C323" s="2"/>
       <c r="D323" s="2"/>
@@ -42463,7 +42436,7 @@
     <row r="324" spans="1:41" ht="14.25" customHeight="1">
       <c r="A324" s="1"/>
       <c r="B324" s="46" t="s">
-        <v>1367</v>
+        <v>788</v>
       </c>
       <c r="C324" s="2"/>
       <c r="D324" s="2"/>
@@ -42569,7 +42542,7 @@
     <row r="325" spans="1:41" ht="14.25" customHeight="1">
       <c r="A325" s="1"/>
       <c r="B325" s="46" t="s">
-        <v>1367</v>
+        <v>788</v>
       </c>
       <c r="C325" s="2"/>
       <c r="D325" s="2"/>
@@ -42675,7 +42648,7 @@
     <row r="326" spans="1:41" ht="14.25" customHeight="1">
       <c r="A326" s="1"/>
       <c r="B326" s="46" t="s">
-        <v>1367</v>
+        <v>788</v>
       </c>
       <c r="C326" s="2"/>
       <c r="D326" s="2"/>
@@ -42778,7 +42751,7 @@
     <row r="327" spans="1:41" ht="14.25" customHeight="1">
       <c r="A327" s="1"/>
       <c r="B327" s="46" t="s">
-        <v>1367</v>
+        <v>788</v>
       </c>
       <c r="C327" s="2"/>
       <c r="D327" s="2"/>
@@ -42881,7 +42854,7 @@
     <row r="328" spans="1:41" ht="14.25" customHeight="1">
       <c r="A328" s="1"/>
       <c r="B328" s="46" t="s">
-        <v>1367</v>
+        <v>788</v>
       </c>
       <c r="C328" s="2"/>
       <c r="D328" s="2"/>
@@ -42984,7 +42957,7 @@
     <row r="329" spans="1:41" ht="14.25" customHeight="1" thickBot="1">
       <c r="A329" s="1"/>
       <c r="B329" s="46" t="s">
-        <v>1367</v>
+        <v>788</v>
       </c>
       <c r="C329" s="2"/>
       <c r="D329" s="2"/>

</xml_diff>

<commit_message>
Changed g to mg for salt
</commit_message>
<xml_diff>
--- a/public/food-data.xlsx
+++ b/public/food-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanau/WebstormProjects/nutrition-calculator/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DDAC5F-C313-8E40-8263-A17F506E1D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EA9828-04D8-2348-AE4F-14DD61059759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5281,30 +5281,30 @@
   <dimension ref="A1:AU1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="N5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AI12" sqref="AI12"/>
+      <selection pane="bottomRight" activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="65.5" hidden="1" customWidth="1"/>
-    <col min="4" max="5" width="8" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="65.5" customWidth="1"/>
+    <col min="4" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="20.1640625" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="9.1640625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="1.83203125" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="6.83203125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" hidden="1" customWidth="1"/>
-    <col min="22" max="29" width="9.1640625" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="15.33203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="15.5" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" customWidth="1"/>
+    <col min="10" max="16" width="9.1640625" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" customWidth="1"/>
+    <col min="18" max="18" width="1.83203125" customWidth="1"/>
+    <col min="19" max="19" width="6.83203125" customWidth="1"/>
+    <col min="20" max="20" width="11.5" customWidth="1"/>
+    <col min="21" max="21" width="12.33203125" customWidth="1"/>
+    <col min="22" max="29" width="9.1640625" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" customWidth="1"/>
     <col min="31" max="31" width="9" customWidth="1"/>
     <col min="32" max="32" width="15.5" customWidth="1"/>
     <col min="33" max="34" width="9" customWidth="1"/>

</xml_diff>